<commit_message>
14 02 2024 +2
</commit_message>
<xml_diff>
--- a/вариант/чайкин/3/22_9871.xlsx
+++ b/вариант/чайкин/3/22_9871.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -33,8 +33,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -118,6 +118,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -196,6 +201,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -230,6 +236,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -405,21 +412,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="62.45" customHeight="1">
+    <row r="1" spans="1:14" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -431,7 +438,7 @@
       </c>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -476,7 +483,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -515,7 +522,7 @@
       </c>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -554,7 +561,7 @@
       </c>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -591,7 +598,7 @@
       </c>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -630,7 +637,7 @@
       </c>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -665,7 +672,7 @@
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -700,7 +707,7 @@
       </c>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -735,7 +742,7 @@
       </c>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -770,7 +777,7 @@
       </c>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -807,7 +814,7 @@
       </c>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -846,7 +853,7 @@
       </c>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -881,7 +888,7 @@
       </c>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -916,7 +923,7 @@
       </c>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -951,7 +958,7 @@
       </c>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -986,7 +993,7 @@
       </c>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1025,7 +1032,7 @@
       </c>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1060,7 +1067,7 @@
       </c>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1095,7 +1102,7 @@
       </c>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1132,7 +1139,7 @@
       </c>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1167,7 +1174,7 @@
       </c>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1204,7 +1211,7 @@
       </c>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1241,7 +1248,7 @@
       </c>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -1280,7 +1287,7 @@
       </c>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -1317,7 +1324,7 @@
       </c>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -1354,7 +1361,7 @@
       </c>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>0</v>
       </c>

</xml_diff>